<commit_message>
Some tests are created and working properly
</commit_message>
<xml_diff>
--- a/OpencartTest/TestData.xlsx
+++ b/OpencartTest/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>bxsfqfuligntaphtnd@ttirv.net</t>
+    <t>qwerty@fhs.com</t>
+  </si>
+  <si>
+    <t>qwerty</t>
+  </si>
+  <si>
+    <t>testing@gmail.com</t>
   </si>
   <si>
     <t>test</t>
@@ -31,7 +37,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,13 +52,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF6A8759"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -76,10 +75,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -366,24 +368,29 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="A2:C3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>